<commit_message>
Improvement of MATLAB Code
Improved the optimization function, and included an optimization
function for the conversion of launch angles to servo angles.

Included changes to the projectile data, by using pixel counters to find
much more accurate and precise launch angle measurements.

Created dedicated folder for competition day.

Created MATLAB competition sketch.
It sorts the target data delivery order such that the cannon will travel
the least amount of distance to minimize operation time.
</commit_message>
<xml_diff>
--- a/MATLAB/Team23_ProjectileData3.xlsx
+++ b/MATLAB/Team23_ProjectileData3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcianus\Documents\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcianus\Documents\GitHub\PingPong-Cannon\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Servo Angle</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>AVG (P = 255)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>AccuLaunchAngle</t>
   </si>
 </sst>
 </file>
@@ -416,66 +422,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D20"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -483,13 +495,19 @@
         <v>25.5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>25.55</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -497,13 +515,19 @@
         <v>28</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>26.98</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -511,13 +535,19 @@
         <v>29.5</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>28.57</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -525,13 +555,19 @@
         <v>30.75</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>30.92</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -539,13 +575,19 @@
         <v>33</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>32.54</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -553,13 +595,19 @@
         <v>35.5</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>35.28</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -567,26 +615,32 @@
         <v>37.5</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>37.71</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D20" si="0">AVERAGE(J8:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E20" si="0">AVERAGE(K8:O8)</f>
         <v>142.25</v>
-      </c>
-      <c r="J8">
-        <v>142</v>
       </c>
       <c r="K8">
         <v>142</v>
       </c>
       <c r="L8">
+        <v>142</v>
+      </c>
+      <c r="M8">
         <v>143</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -594,29 +648,35 @@
         <v>40</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>40.1</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>140.6</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>139</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>140</v>
-      </c>
-      <c r="L9">
-        <v>141</v>
       </c>
       <c r="M9">
         <v>141</v>
       </c>
       <c r="N9">
+        <v>141</v>
+      </c>
+      <c r="O9">
         <v>142</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -624,20 +684,20 @@
         <v>43</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>42.57</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>139.6</v>
       </c>
-      <c r="J10">
-        <v>139</v>
-      </c>
       <c r="K10">
         <v>139</v>
       </c>
       <c r="L10">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M10">
         <v>140</v>
@@ -645,8 +705,14 @@
       <c r="N10">
         <v>140</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>140</v>
+      </c>
+      <c r="Q10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -654,45 +720,51 @@
         <v>45.25</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C24" si="1">AVERAGE(E11:I11)</f>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D24" si="1">AVERAGE(F11:J11)</f>
         <v>122.2</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>138.19999999999999</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>123</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>122</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>121</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>122</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>123</v>
-      </c>
-      <c r="J11">
-        <v>138</v>
       </c>
       <c r="K11">
         <v>138</v>
       </c>
       <c r="L11">
+        <v>138</v>
+      </c>
+      <c r="M11">
         <v>139</v>
-      </c>
-      <c r="M11">
-        <v>138</v>
       </c>
       <c r="N11">
         <v>138</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>138</v>
+      </c>
+      <c r="Q11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -700,16 +772,16 @@
         <v>48.5</v>
       </c>
       <c r="C12">
+        <v>47.59</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>134.4</v>
       </c>
-      <c r="E12">
-        <v>118</v>
-      </c>
       <c r="F12">
         <v>118</v>
       </c>
@@ -723,22 +795,28 @@
         <v>118</v>
       </c>
       <c r="J12">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="K12">
         <v>134</v>
       </c>
       <c r="L12">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M12">
         <v>135</v>
       </c>
       <c r="N12">
+        <v>135</v>
+      </c>
+      <c r="O12">
         <v>134</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -746,21 +824,21 @@
         <v>50.25</v>
       </c>
       <c r="C13">
+        <v>50.2</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="1"/>
         <v>116.2</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>130.4</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>116</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>117</v>
-      </c>
-      <c r="G13">
-        <v>116</v>
       </c>
       <c r="H13">
         <v>116</v>
@@ -769,22 +847,28 @@
         <v>116</v>
       </c>
       <c r="J13">
+        <v>116</v>
+      </c>
+      <c r="K13">
         <v>131</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>130</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>131</v>
-      </c>
-      <c r="M13">
-        <v>130</v>
       </c>
       <c r="N13">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>130</v>
+      </c>
+      <c r="Q13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
@@ -792,45 +876,51 @@
         <v>53</v>
       </c>
       <c r="C14">
+        <v>52.13</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="1"/>
         <v>111.2</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>125.6</v>
       </c>
-      <c r="E14">
-        <v>112</v>
-      </c>
       <c r="F14">
         <v>112</v>
       </c>
       <c r="G14">
+        <v>112</v>
+      </c>
+      <c r="H14">
         <v>110</v>
-      </c>
-      <c r="H14">
-        <v>111</v>
       </c>
       <c r="I14">
         <v>111</v>
       </c>
       <c r="J14">
+        <v>111</v>
+      </c>
+      <c r="K14">
         <v>126</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>125</v>
-      </c>
-      <c r="L14">
-        <v>126</v>
       </c>
       <c r="M14">
         <v>126</v>
       </c>
       <c r="N14">
+        <v>126</v>
+      </c>
+      <c r="O14">
         <v>125</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
@@ -838,18 +928,18 @@
         <v>55.75</v>
       </c>
       <c r="C15">
+        <v>55.32</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="1"/>
         <v>106.2</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>121.6</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>107</v>
-      </c>
-      <c r="F15">
-        <v>106</v>
       </c>
       <c r="G15">
         <v>106</v>
@@ -861,13 +951,13 @@
         <v>106</v>
       </c>
       <c r="J15">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="K15">
         <v>121</v>
       </c>
       <c r="L15">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M15">
         <v>122</v>
@@ -875,8 +965,14 @@
       <c r="N15">
         <v>122</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>122</v>
+      </c>
+      <c r="Q15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -884,30 +980,30 @@
         <v>59</v>
       </c>
       <c r="C16">
+        <v>57.83</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="1"/>
         <v>100.6</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <f t="shared" si="0"/>
         <v>114.8</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>100</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>101</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>100</v>
-      </c>
-      <c r="H16">
-        <v>101</v>
       </c>
       <c r="I16">
         <v>101</v>
       </c>
       <c r="J16">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="K16">
         <v>115</v>
@@ -916,13 +1012,19 @@
         <v>115</v>
       </c>
       <c r="M16">
+        <v>115</v>
+      </c>
+      <c r="N16">
         <v>114</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>115</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
@@ -930,18 +1032,18 @@
         <v>60.5</v>
       </c>
       <c r="C17">
+        <v>59.97</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="1"/>
         <v>96.2</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>108.6</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>97</v>
-      </c>
-      <c r="F17">
-        <v>96</v>
       </c>
       <c r="G17">
         <v>96</v>
@@ -953,22 +1055,28 @@
         <v>96</v>
       </c>
       <c r="J17">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="K17">
         <v>109</v>
       </c>
       <c r="L17">
+        <v>109</v>
+      </c>
+      <c r="M17">
         <v>108</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>109</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
@@ -976,33 +1084,33 @@
         <v>63</v>
       </c>
       <c r="C18">
+        <v>62.5</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>102.2</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>90</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>89</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>90</v>
-      </c>
-      <c r="H18">
-        <v>88</v>
       </c>
       <c r="I18">
         <v>88</v>
       </c>
       <c r="J18">
+        <v>88</v>
+      </c>
+      <c r="K18">
         <v>103</v>
-      </c>
-      <c r="K18">
-        <v>102</v>
       </c>
       <c r="L18">
         <v>102</v>
@@ -1013,8 +1121,14 @@
       <c r="N18">
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>102</v>
+      </c>
+      <c r="Q18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>85</v>
       </c>
@@ -1022,16 +1136,16 @@
         <v>65</v>
       </c>
       <c r="C19">
+        <v>64.34</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <f t="shared" si="0"/>
         <v>94.4</v>
       </c>
-      <c r="E19">
-        <v>83</v>
-      </c>
       <c r="F19">
         <v>83</v>
       </c>
@@ -1045,22 +1159,28 @@
         <v>83</v>
       </c>
       <c r="J19">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="K19">
         <v>94</v>
       </c>
       <c r="L19">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M19">
         <v>95</v>
       </c>
       <c r="N19">
+        <v>95</v>
+      </c>
+      <c r="O19">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90</v>
       </c>
@@ -1068,45 +1188,51 @@
         <v>67.5</v>
       </c>
       <c r="C20">
+        <v>66.97</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="1"/>
         <v>75.2</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <f t="shared" si="0"/>
         <v>84.4</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>76</v>
-      </c>
-      <c r="F20">
-        <v>75</v>
       </c>
       <c r="G20">
         <v>75</v>
       </c>
       <c r="H20">
+        <v>75</v>
+      </c>
+      <c r="I20">
         <v>74</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>76</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>85</v>
-      </c>
-      <c r="K20">
-        <v>84</v>
       </c>
       <c r="L20">
         <v>84</v>
       </c>
       <c r="M20">
+        <v>84</v>
+      </c>
+      <c r="N20">
         <v>85</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>95</v>
       </c>
@@ -1114,20 +1240,20 @@
         <v>69.75</v>
       </c>
       <c r="C21">
+        <v>69.08</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="1"/>
         <v>68.599999999999994</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
       <c r="E21">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>68</v>
       </c>
       <c r="G21">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H21">
         <v>69</v>
@@ -1135,8 +1261,14 @@
       <c r="I21">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>69</v>
+      </c>
+      <c r="Q21">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
@@ -1144,29 +1276,35 @@
         <v>72.5</v>
       </c>
       <c r="C22">
+        <v>70.98</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="1"/>
         <v>60.4</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
       <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <v>60</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>61</v>
-      </c>
-      <c r="G22">
-        <v>60</v>
       </c>
       <c r="H22">
         <v>60</v>
       </c>
       <c r="I22">
+        <v>60</v>
+      </c>
+      <c r="J22">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>105</v>
       </c>
@@ -1174,17 +1312,17 @@
         <v>74</v>
       </c>
       <c r="C23">
+        <v>73.06</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="1"/>
         <v>53.4</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
       <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>54</v>
-      </c>
-      <c r="F23">
-        <v>53</v>
       </c>
       <c r="G23">
         <v>53</v>
@@ -1193,10 +1331,16 @@
         <v>53</v>
       </c>
       <c r="I23">
+        <v>53</v>
+      </c>
+      <c r="J23">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>110</v>
       </c>
@@ -1204,29 +1348,35 @@
         <v>76.5</v>
       </c>
       <c r="C24">
+        <v>75.08</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="1"/>
         <v>47.2</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>48</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>47</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>46</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>47</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>115</v>
       </c>
@@ -1234,13 +1384,19 @@
         <v>77.75</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>76.72</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>120</v>
       </c>
@@ -1248,13 +1404,19 @@
         <v>79.5</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>78.349999999999994</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>125</v>
       </c>
@@ -1262,13 +1424,19 @@
         <v>80.75</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>79.739999999999995</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>130</v>
       </c>
@@ -1276,13 +1444,19 @@
         <v>82</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>81.25</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>135</v>
       </c>
@@ -1290,13 +1464,19 @@
         <v>82.75</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>82.04</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>140</v>
       </c>
@@ -1304,13 +1484,19 @@
         <v>83.5</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>82.3</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>145</v>
       </c>
@@ -1318,13 +1504,19 @@
         <v>84</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>83.33</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>150</v>
       </c>
@@ -1332,13 +1524,19 @@
         <v>83.5</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>82.98</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>155</v>
       </c>
@@ -1346,13 +1544,19 @@
         <v>83.25</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>82.56</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>160</v>
       </c>
@@ -1360,13 +1564,19 @@
         <v>82.5</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>82.13</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>165</v>
       </c>
@@ -1374,13 +1584,19 @@
         <v>81.5</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>82.24</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>170</v>
       </c>
@@ -1388,13 +1604,19 @@
         <v>80.5</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>80.72</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>175</v>
       </c>
@@ -1402,13 +1624,19 @@
         <v>78.5</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>78.17</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>180</v>
       </c>
@@ -1416,10 +1644,16 @@
         <v>76.5</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>76.209999999999994</v>
       </c>
       <c r="D38">
         <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perfecting Code for Competition
Added horizontal offsets to compensate for consistently shooting to the
right.
Also recalibrated based on new launcher data.
When the cannon is already home, and the returnHome() function gets
called, it will just return zero, rather than attempting to move.
</commit_message>
<xml_diff>
--- a/MATLAB/Team23_ProjectileData3.xlsx
+++ b/MATLAB/Team23_ProjectileData3.xlsx
@@ -425,7 +425,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="C11" sqref="A11:C11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +720,7 @@
         <v>45.25</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>45.25</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D24" si="1">AVERAGE(F11:J11)</f>

</xml_diff>